<commit_message>
RCP-Qlearning now matches the theoretical result
1. fix an error in RTT-Variance calculation
2. fix corresponding errors in the theoretical calculation because of the error in 1.
3. fix the mistake of failed to normalize the delay when calculating expected delay
</commit_message>
<xml_diff>
--- a/summary_v_n_s.xlsx
+++ b/summary_v_n_s.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuwang/Github/RCP-Ver2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE50C21-DB0D-9A44-AEE7-0C300958E2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28C6DB5-C397-FC42-B5BD-863091CDF889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="4360" windowWidth="51200" windowHeight="25640" xr2:uid="{18D2911A-C427-4948-895E-F5C1AAE63140}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21660" xr2:uid="{18D2911A-C427-4948-895E-F5C1AAE63140}"/>
   </bookViews>
   <sheets>
     <sheet name="case_study" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{69A84B6E-E790-8442-AD71-9058C1676C0B}" name="RTQ_s" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="2" sourceFile="/Users/yuwang/Github/RCP-Ver2/Results/case_study_TimeDiscount_alpha_2_0/summary/RTQ_s.txt" comma="1">
+    <textPr firstRow="2" sourceFile="/Users/yuwang/Github/RCP-Ver2/Results/case_study_TimeDiscount_alpha_2_0/summary/RTQ_s.txt" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -128,7 +128,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{C1AA26BB-0FF8-DA40-AFCA-E532A0A473C2}" name="RTQ_v" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/yuwang/Github/RCP-Ver2/Results/case_study_TimeDiscount_alpha_2_0/summary/RTQ_v.txt" comma="1">
+    <textPr sourceFile="/Users/yuwang/Github/RCP-Ver2/Results/case_study_TimeDiscount_alpha_2_0/summary/RTQ_v.txt" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -323,13 +323,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -350,15 +350,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RTQ_v" connectionId="6" xr16:uid="{1819C5A7-5CE6-F944-AF94-40D5131AB08E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RTQ_s" connectionId="5" xr16:uid="{BDB40988-101F-B14E-9105-BE89FF154906}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="theore_v" connectionId="9" xr16:uid="{67AFF46D-E563-5448-9E28-04F6B1B0F481}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RTQ_v" connectionId="6" xr16:uid="{1819C5A7-5CE6-F944-AF94-40D5131AB08E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="theore_s_2" connectionId="8" xr16:uid="{52B12F4C-A94A-F74A-97FF-14F205E59E71}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,27 +366,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="theore_s_1" connectionId="7" xr16:uid="{65576909-2375-A34B-A7AB-4B201D13E7EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Q_learning_v_2" connectionId="4" xr16:uid="{0A2B2617-1F64-C84C-B22B-A63BA2401ECA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Q_learning_s_1" connectionId="1" xr16:uid="{59CC6985-2B4D-E848-A31B-A5E7B1292291}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="theore_v" connectionId="9" xr16:uid="{67AFF46D-E563-5448-9E28-04F6B1B0F481}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Q_learning_v_1" connectionId="3" xr16:uid="{5E436E21-E9D8-0047-A075-BA372CF44888}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="theore_v_1" connectionId="10" xr16:uid="{0FBB104C-262B-034D-837D-2CB458DFA23A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="theore_s_2" connectionId="8" xr16:uid="{52B12F4C-A94A-F74A-97FF-14F205E59E71}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="theore_s_1" connectionId="7" xr16:uid="{65576909-2375-A34B-A7AB-4B201D13E7EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Q_learning_v_2" connectionId="4" xr16:uid="{0A2B2617-1F64-C84C-B22B-A63BA2401ECA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73DA64E-AC48-3440-AD24-59B38083828D}">
   <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,7 +701,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="34" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="4"/>
@@ -742,45 +742,45 @@
       <c r="AK1" s="4"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="N2" s="3" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="AA2" s="3" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="AA2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1030,30 +1030,14 @@
       <c r="AA5" s="1">
         <v>2</v>
       </c>
-      <c r="AB5" s="2">
-        <v>2.3309E-2</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>6.7458000000000004E-2</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>0.113773</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>0.171371</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>0.20419799999999999</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>0.26779399999999998</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>0.31565799999999999</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>0.43198900000000001</v>
-      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
       <c r="AJ5" s="2">
         <v>0.69029300000000005</v>
       </c>
@@ -1103,33 +1087,15 @@
       <c r="AA6" s="1">
         <v>3</v>
       </c>
-      <c r="AB6" s="2">
-        <v>2.7886999999999999E-2</v>
-      </c>
-      <c r="AC6" s="2">
-        <v>6.7221000000000003E-2</v>
-      </c>
-      <c r="AD6" s="2">
-        <v>0.10499600000000001</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>0.15521499999999999</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>0.240844</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>0.23330300000000001</v>
-      </c>
-      <c r="AH6" s="2">
-        <v>0.29891800000000002</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>0.45150699999999999</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>0.68517799999999995</v>
-      </c>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
       <c r="AK6" s="2">
         <v>1.111103</v>
       </c>
@@ -1172,33 +1138,15 @@
       <c r="AA7" s="1">
         <v>4</v>
       </c>
-      <c r="AB7" s="2">
-        <v>2.0518999999999999E-2</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>5.2533999999999997E-2</v>
-      </c>
-      <c r="AD7" s="2">
-        <v>0.10194</v>
-      </c>
-      <c r="AE7" s="2">
-        <v>0.14086899999999999</v>
-      </c>
-      <c r="AF7" s="2">
-        <v>0.214721</v>
-      </c>
-      <c r="AG7" s="2">
-        <v>0.26921499999999998</v>
-      </c>
-      <c r="AH7" s="2">
-        <v>0.362041</v>
-      </c>
-      <c r="AI7" s="2">
-        <v>0.432861</v>
-      </c>
-      <c r="AJ7" s="2">
-        <v>0.73912500000000003</v>
-      </c>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
       <c r="AK7" s="2">
         <v>1.1110260000000001</v>
       </c>
@@ -1241,33 +1189,15 @@
       <c r="AA8" s="1">
         <v>5</v>
       </c>
-      <c r="AB8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="2">
-        <v>0</v>
-      </c>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
       <c r="AK8" s="2">
         <v>1.1102590000000001</v>
       </c>
@@ -1306,33 +1236,15 @@
       <c r="AA9" s="1">
         <v>6</v>
       </c>
-      <c r="AB9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="2">
-        <v>0</v>
-      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
       <c r="AK9" s="2">
         <v>1.1025879999999999</v>
       </c>
@@ -1371,36 +1283,16 @@
       <c r="AA10" s="1">
         <v>7</v>
       </c>
-      <c r="AB10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="2">
-        <v>1.0258849999999999</v>
-      </c>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1852,32 +1744,32 @@
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="N24" s="3" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="N24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">

</xml_diff>